<commit_message>
Updating 4.Recycling, Extraction of material recycled for each component
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,37 +11783,37 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1336</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1342</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1340</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1337</v>
+        <v>1341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shock for SG2 and FD
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11788,27 +11788,27 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1336</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1337</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1339</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>

<commit_message>
Fixing name of Sectors to be alligned with Baseline
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,37 +11783,37 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1339</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1336</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempt to create scenarios
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,7 +11783,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -11793,27 +11793,27 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1338</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improving calc shocks in 6.Add wastw sectors.py
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,37 +11783,37 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1336</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1341</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1337</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change in unit of AIC and run of new results
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,37 +11783,37 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1339</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1336</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1337</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing coefficients of recycling in A2 + correcting equation of EoL
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,17 +11783,17 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1338</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -11803,17 +11803,17 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1341</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creation allocation matrix for dMRWIO + Results_region
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,37 +11783,37 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1337</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1341</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run to extract data to excel
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,17 +11783,17 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1338</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1342</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -11803,17 +11803,17 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1336</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set up Scenarios + sensitivity scripts and first run
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,37 +11783,37 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1342</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1340</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1336</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Final Demand projection
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11783,7 +11783,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1336</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -11793,27 +11793,27 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1337</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculation of EOL RIR inidcator
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11789,12 +11789,12 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -11804,22 +11804,22 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1338</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1341</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Share consumption of region for Green Technologies
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11789,22 +11789,22 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -11819,7 +11819,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run sensitivity lifetime + plot share
</commit_message>
<xml_diff>
--- a/Add Sectors/new_waste_sector.xlsx
+++ b/Add Sectors/new_waste_sector.xlsx
@@ -11789,37 +11789,37 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1340</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>1338</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>